<commit_message>
Removed 0945.HK ManuLife from IPO 2018 Reform
</commit_message>
<xml_diff>
--- a/HKEX_List_1999.xlsx
+++ b/HKEX_List_1999.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\GitHub\exchatbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47526046-1980-4FEC-BAF9-E9D5A1D1CA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAAC607-9DC9-439C-99B3-256E05ADE087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6179" uniqueCount="2538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6178" uniqueCount="2537">
   <si>
     <t>Ticker</t>
   </si>
@@ -7634,9 +7634,6 @@
   </si>
   <si>
     <t>REFORM_BSW</t>
-  </si>
-  <si>
-    <t>S</t>
   </si>
 </sst>
 </file>
@@ -8493,7 +8490,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P609"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -31520,9 +31519,6 @@
       <c r="F490" t="s">
         <v>1919</v>
       </c>
-      <c r="G490" t="s">
-        <v>2537</v>
-      </c>
       <c r="H490" t="s">
         <v>1926</v>
       </c>

</xml_diff>